<commit_message>
Add info for test results
</commit_message>
<xml_diff>
--- a/blogs/test_extension/user_test_results.xlsx
+++ b/blogs/test_extension/user_test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d074144\Workspace\DH\fridgify-doc\blogs\test_extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF42D385-A103-4EBA-BE16-B178E6A0DB3C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A2B930-582E-4F86-A5F8-D16ACABC03C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E80BA7E-A9B2-4916-AC74-69FC4DFC9EE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E80BA7E-A9B2-4916-AC74-69FC4DFC9EE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Login/Register</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Change items of a fidge</t>
+  </si>
+  <si>
+    <t>&lt;- Rounded sum of all values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculated by hand. Survey tool of choice was not that advanced. My bad on that one. </t>
   </si>
 </sst>
 </file>
@@ -3491,15 +3497,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
+      <xdr:colOff>276224</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
+      <xdr:colOff>114299</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3932,10 +3938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D80E0A-5E89-4D95-8BC7-4EE2E3612485}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3947,7 +3953,7 @@
     <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3961,7 +3967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3977,8 +3983,11 @@
       <c r="E2">
         <v>2</v>
       </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3994,8 +4003,11 @@
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>

</xml_diff>